<commit_message>
Updates to EMEP inventories Misc. updates for debugging purposes
</commit_message>
<xml_diff>
--- a/input/activity/metals/Blast furnace iron production, 1980-2017.xlsx
+++ b/input/activity/metals/Blast furnace iron production, 1980-2017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/activity/metals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C8951B6-0D4E-D940-8E4E-02B0D9437D49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA66BB05-1289-4C4D-BA90-819300DFE06B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="1280" windowWidth="25600" windowHeight="16060" tabRatio="204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,14 @@
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -750,13 +756,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AJ95"/>
+  <dimension ref="A1:AM95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AC42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
+      <selection pane="bottomRight" activeCell="AK67" sqref="AK67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,9 +771,10 @@
     <col min="2" max="2" width="5.6640625" customWidth="1"/>
     <col min="3" max="31" width="8.1640625" customWidth="1"/>
     <col min="32" max="36" width="9.83203125" customWidth="1"/>
+    <col min="37" max="39" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -776,12 +783,12 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -890,8 +897,17 @@
       <c r="AJ3" s="1">
         <v>2014</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK3" s="1">
+        <v>2015</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -957,7 +973,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1066,8 +1082,17 @@
       <c r="AJ5" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK5" s="2">
+        <v>300</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>300</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1176,8 +1201,17 @@
       <c r="AJ6" s="2">
         <v>2766</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK6" s="2">
+        <v>2685</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>2141</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1286,8 +1320,17 @@
       <c r="AJ7" s="2">
         <v>3282</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK7" s="2">
+        <v>3594</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>3642</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1396,8 +1439,17 @@
       <c r="AJ8" s="2">
         <v>6029</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK8" s="2">
+        <v>5805</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>5642</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>6335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1506,8 +1558,17 @@
       <c r="AJ9" s="2">
         <v>4388</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK9" s="2">
+        <v>4248</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>4869</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>4860</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1560,8 +1621,17 @@
       <c r="AJ10" s="2">
         <v>860</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK10" s="2">
+        <v>845</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>778</v>
+      </c>
+      <c r="AM10" s="2">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1670,8 +1740,17 @@
       <c r="AJ11" s="2">
         <v>27016</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK11" s="2">
+        <v>27803</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>26036</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>28427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1769,7 +1848,7 @@
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1878,8 +1957,17 @@
       <c r="AJ13" s="2">
         <v>6728</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK13" s="2">
+        <v>5851</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>6240</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1988,8 +2076,17 @@
       <c r="AJ14" s="2">
         <v>584</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK14" s="2">
+        <v>644</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>677</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2098,8 +2195,17 @@
       <c r="AJ15" s="2">
         <v>711600</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK15" s="2">
+        <v>691413</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>698190</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>710760</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2208,8 +2314,17 @@
       <c r="AJ16" s="2">
         <v>234</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK16" s="2">
+        <v>240</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>225</v>
+      </c>
+      <c r="AM16" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2294,8 +2409,17 @@
       <c r="AJ17" s="2">
         <v>4152</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK17" s="2">
+        <v>4031</v>
+      </c>
+      <c r="AL17" s="2">
+        <v>4165</v>
+      </c>
+      <c r="AM17" s="2">
+        <v>3691</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2483,7 @@
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2468,8 +2592,17 @@
       <c r="AJ19" s="2">
         <v>550</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK19" s="2">
+        <v>500</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>500</v>
+      </c>
+      <c r="AM19" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2541,7 +2674,7 @@
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2650,8 +2783,17 @@
       <c r="AJ21" s="2">
         <v>2475</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK21" s="2">
+        <v>2594</v>
+      </c>
+      <c r="AL21" s="2">
+        <v>2670</v>
+      </c>
+      <c r="AM21" s="2">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2760,8 +2902,17 @@
       <c r="AJ22" s="2">
         <v>10866</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK22" s="2">
+        <v>10097</v>
+      </c>
+      <c r="AL22" s="2">
+        <v>9724</v>
+      </c>
+      <c r="AM22" s="2">
+        <v>10678</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2870,8 +3021,17 @@
       <c r="AJ23" s="2">
         <v>27379</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK23" s="2">
+        <v>27842</v>
+      </c>
+      <c r="AL23" s="2">
+        <v>27270</v>
+      </c>
+      <c r="AM23" s="2">
+        <v>27816</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +3093,7 @@
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3042,8 +3202,17 @@
       <c r="AJ25" s="2">
         <v>801</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK25" s="2">
+        <v>1247</v>
+      </c>
+      <c r="AL25" s="2">
+        <v>864</v>
+      </c>
+      <c r="AM25" s="2">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3152,8 +3321,17 @@
       <c r="AJ26" s="2">
         <v>55166</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK26" s="2">
+        <v>58394</v>
+      </c>
+      <c r="AL26" s="2">
+        <v>63714</v>
+      </c>
+      <c r="AM26" s="2">
+        <v>66808</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3262,8 +3440,17 @@
       <c r="AJ27" s="2">
         <v>2782</v>
       </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK27" s="2">
+        <v>2459</v>
+      </c>
+      <c r="AL27" s="2">
+        <v>2251</v>
+      </c>
+      <c r="AM27" s="2">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3372,8 +3559,17 @@
       <c r="AJ28" s="2">
         <v>6371</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK28" s="2">
+        <v>5051</v>
+      </c>
+      <c r="AL28" s="2">
+        <v>6044</v>
+      </c>
+      <c r="AM28" s="2">
+        <v>5052</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3482,8 +3678,17 @@
       <c r="AJ29" s="2">
         <v>83872</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK29" s="2">
+        <v>81011</v>
+      </c>
+      <c r="AL29" s="2">
+        <v>80186</v>
+      </c>
+      <c r="AM29" s="2">
+        <v>78330</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3568,8 +3773,17 @@
       <c r="AJ30" s="2">
         <v>3185</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK30" s="2">
+        <v>3235</v>
+      </c>
+      <c r="AL30" s="2">
+        <v>6901</v>
+      </c>
+      <c r="AM30" s="2">
+        <v>3769</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3645,7 +3859,7 @@
       <c r="AI31" s="2"/>
       <c r="AJ31" s="2"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -3716,8 +3930,17 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
       <c r="AJ32" s="2"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK32" s="2">
+        <v>477</v>
+      </c>
+      <c r="AL32" s="2">
+        <v>522</v>
+      </c>
+      <c r="AM32" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -3826,8 +4049,17 @@
       <c r="AJ33" s="2">
         <v>5116</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK33" s="2">
+        <v>4573</v>
+      </c>
+      <c r="AL33" s="2">
+        <v>4476</v>
+      </c>
+      <c r="AM33" s="2">
+        <v>4245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -3913,7 +4145,7 @@
       <c r="AI34" s="2"/>
       <c r="AJ34" s="2"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -4022,8 +4254,17 @@
       <c r="AJ35" s="2">
         <v>5868</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK35" s="2">
+        <v>6050</v>
+      </c>
+      <c r="AL35" s="2">
+        <v>6092</v>
+      </c>
+      <c r="AM35" s="2">
+        <v>6145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4116,8 +4357,17 @@
       <c r="AJ36" s="2">
         <v>680</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK36" s="2">
+        <v>678</v>
+      </c>
+      <c r="AL36" s="2">
+        <v>670</v>
+      </c>
+      <c r="AM36" s="2">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -4226,8 +4476,17 @@
       <c r="AJ37" s="2">
         <v>250</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK37" s="2">
+        <v>250</v>
+      </c>
+      <c r="AL37" s="2">
+        <v>250</v>
+      </c>
+      <c r="AM37" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4336,8 +4595,17 @@
       <c r="AJ38" s="2">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK38" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL38" s="2">
+        <v>100</v>
+      </c>
+      <c r="AM38" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4444,8 +4712,11 @@
       <c r="AJ39" s="2">
         <v>142</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK39" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4540,8 +4811,17 @@
       <c r="AJ40" s="2">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK40" s="2">
+        <v>73</v>
+      </c>
+      <c r="AL40" s="2">
+        <v>50</v>
+      </c>
+      <c r="AM40" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -4630,7 +4910,7 @@
         <v>351</v>
       </c>
       <c r="AD41" s="2">
-        <v>412</v>
+        <v>345</v>
       </c>
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
@@ -4639,7 +4919,7 @@
       <c r="AI41" s="2"/>
       <c r="AJ41" s="2"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -4748,8 +5028,17 @@
       <c r="AJ42" s="2">
         <v>4637</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK42" s="2">
+        <v>4821</v>
+      </c>
+      <c r="AL42" s="2">
+        <v>4674</v>
+      </c>
+      <c r="AM42" s="2">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -4833,7 +5122,7 @@
       <c r="AI43" s="2"/>
       <c r="AJ43" s="2"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -4942,8 +5231,17 @@
       <c r="AJ44" s="2">
         <v>1631</v>
       </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK44" s="2">
+        <v>1983</v>
+      </c>
+      <c r="AL44" s="2">
+        <v>1972</v>
+      </c>
+      <c r="AM44" s="2">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -5028,8 +5326,17 @@
       <c r="AJ45" s="2">
         <v>51479</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK45" s="2">
+        <v>52553</v>
+      </c>
+      <c r="AL45" s="2">
+        <v>51877</v>
+      </c>
+      <c r="AM45" s="2">
+        <v>52036</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -5093,7 +5400,7 @@
       <c r="AI46" s="2"/>
       <c r="AJ46" s="2"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -5146,8 +5453,17 @@
       <c r="AJ47" s="2">
         <v>550</v>
       </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK47" s="2">
+        <v>904</v>
+      </c>
+      <c r="AL47" s="2">
+        <v>1154</v>
+      </c>
+      <c r="AM47" s="2">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -5232,8 +5548,17 @@
       <c r="AJ48" s="2">
         <v>3838</v>
       </c>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK48" s="2">
+        <v>3738</v>
+      </c>
+      <c r="AL48" s="2">
+        <v>3987</v>
+      </c>
+      <c r="AM48" s="2">
+        <v>4106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -5340,10 +5665,19 @@
         <v>4928</v>
       </c>
       <c r="AJ49" s="2">
-        <v>4690</v>
-      </c>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+        <v>4402</v>
+      </c>
+      <c r="AK49" s="2">
+        <v>4464</v>
+      </c>
+      <c r="AL49" s="2">
+        <v>4311</v>
+      </c>
+      <c r="AM49" s="2">
+        <v>4352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -5452,8 +5786,17 @@
       <c r="AJ50" s="2">
         <v>46909</v>
       </c>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK50" s="2">
+        <v>47639</v>
+      </c>
+      <c r="AL50" s="2">
+        <v>46336</v>
+      </c>
+      <c r="AM50" s="2">
+        <v>47071</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -5562,8 +5905,17 @@
       <c r="AJ51" s="2">
         <v>3958</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK51" s="2">
+        <v>4450</v>
+      </c>
+      <c r="AL51" s="2">
+        <v>4116</v>
+      </c>
+      <c r="AM51" s="2">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -5672,8 +6024,17 @@
       <c r="AJ52" s="2">
         <v>3078</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK52" s="2">
+        <v>2865</v>
+      </c>
+      <c r="AL52" s="2">
+        <v>3079</v>
+      </c>
+      <c r="AM52" s="2">
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -5757,7 +6118,7 @@
       <c r="AI53" s="2"/>
       <c r="AJ53" s="2"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -5866,8 +6227,17 @@
       <c r="AJ54" s="2">
         <v>14440</v>
       </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK54" s="2">
+        <v>14370</v>
+      </c>
+      <c r="AL54" s="2">
+        <v>14890</v>
+      </c>
+      <c r="AM54" s="2">
+        <v>14361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -5955,7 +6325,7 @@
       <c r="AI55" s="2"/>
       <c r="AJ55" s="2"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -6064,8 +6434,17 @@
       <c r="AJ56" s="2">
         <v>9364</v>
       </c>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK56" s="2">
+        <v>10184</v>
+      </c>
+      <c r="AL56" s="2">
+        <v>10304</v>
+      </c>
+      <c r="AM56" s="2">
+        <v>10589</v>
+      </c>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -6150,8 +6529,17 @@
       <c r="AJ57" s="2">
         <v>24788</v>
       </c>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK57" s="2">
+        <v>21797</v>
+      </c>
+      <c r="AL57" s="2">
+        <v>23618</v>
+      </c>
+      <c r="AM57" s="2">
+        <v>20123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -6260,8 +6648,17 @@
       <c r="AJ58" s="2">
         <v>9705</v>
       </c>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK58" s="2">
+        <v>8774</v>
+      </c>
+      <c r="AL58" s="2">
+        <v>6142</v>
+      </c>
+      <c r="AM58" s="2">
+        <v>5996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -6370,8 +6767,17 @@
       <c r="AJ59" s="2">
         <v>29374</v>
       </c>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK59" s="2">
+        <v>25435</v>
+      </c>
+      <c r="AL59" s="2">
+        <v>22293</v>
+      </c>
+      <c r="AM59" s="2">
+        <v>22395</v>
+      </c>
+    </row>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -6433,7 +6839,7 @@
       <c r="AI60" s="2"/>
       <c r="AJ60" s="2"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -6518,8 +6924,17 @@
       <c r="AJ61" s="2">
         <v>1393</v>
       </c>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK61" s="2">
+        <v>1700</v>
+      </c>
+      <c r="AL61" s="2">
+        <v>2600</v>
+      </c>
+      <c r="AM61" s="2">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -6583,7 +6998,7 @@
       <c r="AI62" s="2"/>
       <c r="AJ62" s="2"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
@@ -6679,7 +7094,7 @@
       <c r="AI63" s="4"/>
       <c r="AJ63" s="4"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -6786,10 +7201,19 @@
         <v>1206676</v>
       </c>
       <c r="AJ64" s="2">
-        <v>1183451</v>
-      </c>
-    </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
+        <v>1185311</v>
+      </c>
+      <c r="AK64" s="2">
+        <v>1157930</v>
+      </c>
+      <c r="AL64" s="2">
+        <v>1166545</v>
+      </c>
+      <c r="AM64" s="2">
+        <v>1180494</v>
+      </c>
+    </row>
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -6826,7 +7250,7 @@
       <c r="AI65" s="2"/>
       <c r="AJ65" s="2"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -6935,8 +7359,17 @@
       <c r="AJ66" s="2">
         <v>2014</v>
       </c>
-    </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK66" s="2">
+        <v>2015</v>
+      </c>
+      <c r="AL66" s="2">
+        <v>2016</v>
+      </c>
+      <c r="AM66" s="2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -6976,7 +7409,7 @@
       <c r="AI67" s="2"/>
       <c r="AJ67" s="2"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -7074,19 +7507,35 @@
         <v>64523</v>
       </c>
       <c r="AG68" s="2">
+        <f>AG9+AG22+AG23+AG28+AG31+AG35+AG58</f>
         <v>64392</v>
       </c>
       <c r="AH68" s="2">
-        <v>62623</v>
+        <f>AH9+AH22+AH23+AH28+AH31+AH35+AH58</f>
+        <v>62622</v>
       </c>
       <c r="AI68" s="2">
-        <v>63381</v>
+        <f>AI9+AI22+AI23+AI28+AI31+AI35+AI58</f>
+        <v>63382</v>
       </c>
       <c r="AJ68" s="2">
-        <v>64575</v>
-      </c>
-    </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
+        <f>AJ9+AJ22+AJ23+AJ28+AJ31+AJ35+AJ58</f>
+        <v>64577</v>
+      </c>
+      <c r="AK68" s="2">
+        <f>AK9+AK22+AK23+AK28+AK31+AK35+AK58</f>
+        <v>62062</v>
+      </c>
+      <c r="AL68" s="2">
+        <f>AL9+AL22+AL23+AL28+AL31+AL35+AL58</f>
+        <v>60141</v>
+      </c>
+      <c r="AM68" s="2">
+        <f>AM9+AM22+AM23+AM28+AM31+AM35+AM58</f>
+        <v>60547</v>
+      </c>
+    </row>
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -7184,19 +7633,35 @@
         <v>68096</v>
       </c>
       <c r="AG69" s="2">
+        <f>AG68+AG43+AG51</f>
         <v>67932</v>
       </c>
       <c r="AH69" s="2">
-        <v>65704</v>
+        <f>AH68+AH43+AH51</f>
+        <v>65703</v>
       </c>
       <c r="AI69" s="2">
-        <v>67330</v>
+        <f>AI68+AI43+AI51</f>
+        <v>67331</v>
       </c>
       <c r="AJ69" s="2">
-        <v>68534</v>
-      </c>
-    </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
+        <f>AJ68+AJ43+AJ51</f>
+        <v>68535</v>
+      </c>
+      <c r="AK69" s="2">
+        <f>AK68+AK43+AK51</f>
+        <v>66512</v>
+      </c>
+      <c r="AL69" s="2">
+        <f>AL68+AL43+AL51</f>
+        <v>64257</v>
+      </c>
+      <c r="AM69" s="2">
+        <f>AM68+AM43+AM51</f>
+        <v>65009</v>
+      </c>
+    </row>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -7294,19 +7759,35 @@
         <v>79729</v>
       </c>
       <c r="AG70" s="2">
+        <f>AG69+AG8+AG21+AG52</f>
         <v>79487</v>
       </c>
       <c r="AH70" s="2">
-        <v>76390</v>
+        <f>AH69+AH8+AH21+AH52</f>
+        <v>76389</v>
       </c>
       <c r="AI70" s="2">
-        <v>78428</v>
+        <f>AI69+AI8+AI21+AI52</f>
+        <v>78429</v>
       </c>
       <c r="AJ70" s="2">
-        <v>80116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
+        <f>AJ69+AJ8+AJ21+AJ52</f>
+        <v>80117</v>
+      </c>
+      <c r="AK70" s="2">
+        <f>AK69+AK8+AK21+AK52</f>
+        <v>77776</v>
+      </c>
+      <c r="AL70" s="2">
+        <f>AL69+AL8+AL21+AL52</f>
+        <v>75648</v>
+      </c>
+      <c r="AM70" s="2">
+        <f>AM69+AM8+AM21+AM52</f>
+        <v>77059</v>
+      </c>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -7404,19 +7885,35 @@
         <v>92328</v>
       </c>
       <c r="AG71" s="2">
+        <f>AG70+AG17+AG25+AG42+AG48</f>
         <v>92262</v>
       </c>
       <c r="AH71" s="2">
-        <v>89026</v>
+        <f>AH70+AH17+AH25+AH42+AH48</f>
+        <v>89025</v>
       </c>
       <c r="AI71" s="2">
-        <v>90724</v>
+        <f>AI70+AI17+AI25+AI42+AI48</f>
+        <v>90725</v>
       </c>
       <c r="AJ71" s="2">
+        <f>AJ70+AJ17+AJ25+AJ42+AJ48</f>
         <v>93545</v>
       </c>
-    </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK71" s="2">
+        <f>AK70+AK17+AK25+AK42+AK48</f>
+        <v>91613</v>
+      </c>
+      <c r="AL71" s="2">
+        <f>AL70+AL17+AL25+AL42+AL48</f>
+        <v>89338</v>
+      </c>
+      <c r="AM71" s="2">
+        <f>AM70+AM17+AM25+AM42+AM48</f>
+        <v>91318</v>
+      </c>
+    </row>
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -7525,8 +8022,17 @@
       <c r="AJ72" s="2">
         <v>95176</v>
       </c>
-    </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK72" s="2">
+        <v>93596</v>
+      </c>
+      <c r="AL72" s="2">
+        <v>91312</v>
+      </c>
+      <c r="AM72" s="2">
+        <v>93246</v>
+      </c>
+    </row>
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -7611,8 +8117,17 @@
       <c r="AJ73" s="2">
         <v>79452</v>
       </c>
-    </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK73" s="2">
+        <v>77585</v>
+      </c>
+      <c r="AL73" s="2">
+        <v>82396</v>
+      </c>
+      <c r="AM73" s="2">
+        <v>75928</v>
+      </c>
+    </row>
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>45</v>
       </c>
@@ -7721,8 +8236,17 @@
       <c r="AJ74" s="2">
         <v>79452</v>
       </c>
-    </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK74" s="2">
+        <v>77585</v>
+      </c>
+      <c r="AL74" s="2">
+        <v>82396</v>
+      </c>
+      <c r="AM74" s="2">
+        <v>75928</v>
+      </c>
+    </row>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -7829,10 +8353,19 @@
         <v>41319</v>
       </c>
       <c r="AJ75" s="2">
-        <v>41219</v>
-      </c>
-    </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
+        <v>41218</v>
+      </c>
+      <c r="AK75" s="2">
+        <v>35859</v>
+      </c>
+      <c r="AL75" s="2">
+        <v>33008</v>
+      </c>
+      <c r="AM75" s="2">
+        <v>32946</v>
+      </c>
+    </row>
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -7941,8 +8474,17 @@
       <c r="AJ76" s="2">
         <v>30671</v>
       </c>
-    </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK76" s="2">
+        <v>31446</v>
+      </c>
+      <c r="AL76" s="2">
+        <v>29130</v>
+      </c>
+      <c r="AM76" s="2">
+        <v>31509</v>
+      </c>
+    </row>
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -8049,10 +8591,19 @@
         <v>5778</v>
       </c>
       <c r="AJ77" s="2">
-        <v>5540</v>
-      </c>
-    </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
+        <v>5252</v>
+      </c>
+      <c r="AK77" s="2">
+        <v>5264</v>
+      </c>
+      <c r="AL77" s="2">
+        <v>5111</v>
+      </c>
+      <c r="AM77" s="2">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -8161,8 +8712,17 @@
       <c r="AJ78" s="2">
         <v>2782</v>
       </c>
-    </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK78" s="2">
+        <v>2459</v>
+      </c>
+      <c r="AL78" s="2">
+        <v>2251</v>
+      </c>
+      <c r="AM78" s="2">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -8269,10 +8829,19 @@
         <v>942881</v>
       </c>
       <c r="AJ79" s="2">
-        <v>917734</v>
-      </c>
-    </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
+        <v>919883</v>
+      </c>
+      <c r="AK79" s="2">
+        <v>899687</v>
+      </c>
+      <c r="AL79" s="2">
+        <v>911000</v>
+      </c>
+      <c r="AM79" s="2">
+        <v>926653</v>
+      </c>
+    </row>
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -8379,10 +8948,19 @@
         <v>458592</v>
       </c>
       <c r="AJ80" s="2">
-        <v>471851</v>
-      </c>
-    </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+        <v>471563</v>
+      </c>
+      <c r="AK80" s="2">
+        <v>466517</v>
+      </c>
+      <c r="AL80" s="2">
+        <v>468355</v>
+      </c>
+      <c r="AM80" s="2">
+        <v>469734</v>
+      </c>
+    </row>
+    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>63</v>
       </c>
@@ -8489,16 +9067,25 @@
         <v>1206676</v>
       </c>
       <c r="AJ81" s="2">
-        <v>1183451</v>
-      </c>
-    </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+        <v>1185311</v>
+      </c>
+      <c r="AK81" s="2">
+        <v>1157930</v>
+      </c>
+      <c r="AL81" s="2">
+        <v>1166545</v>
+      </c>
+      <c r="AM81" s="2">
+        <v>1180494</v>
+      </c>
+    </row>
+    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>66</v>
       </c>
@@ -8506,7 +9093,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>67</v>
       </c>
@@ -8514,7 +9101,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>68</v>
       </c>
@@ -8522,7 +9109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>69</v>
       </c>
@@ -8530,7 +9117,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>70</v>
       </c>
@@ -8538,7 +9125,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>71</v>
       </c>
@@ -8546,7 +9133,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>45</v>
       </c>
@@ -8554,7 +9141,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>72</v>
       </c>
@@ -8562,7 +9149,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>73</v>
       </c>
@@ -8570,7 +9157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>74</v>
       </c>
@@ -8578,7 +9165,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>75</v>
       </c>
@@ -8586,7 +9173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>76</v>
       </c>

</xml_diff>